<commit_message>
daily-log as pandas was not working to update excel, change to list of rows
</commit_message>
<xml_diff>
--- a/Nutrition/FoodDictionary.xlsx
+++ b/Nutrition/FoodDictionary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kobi Cohen\PycharmProjects\NutritionLog\Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C07C86D-9933-4B0B-84D5-BAC0227AC587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E39FC-1E89-45CF-B4A4-351D245E3D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="1170" yWindow="750" windowWidth="17295" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodDictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Food</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Calories</t>
   </si>
   <si>
@@ -238,16 +235,13 @@
     <t>protein bar</t>
   </si>
   <si>
-    <t>חטיף חלבון</t>
-  </si>
-  <si>
-    <t>יחידה</t>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1081,19 +1075,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,30 +1095,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>65</v>
@@ -1139,15 +1133,15 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>127</v>
@@ -1162,15 +1156,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>114</v>
@@ -1185,15 +1179,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5">
         <v>30.85</v>
@@ -1208,15 +1202,15 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>745</v>
@@ -1231,15 +1225,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
       <c r="D7">
         <v>66</v>
@@ -1254,15 +1248,15 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>1.5</v>
@@ -1277,15 +1271,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>8.34</v>
@@ -1300,15 +1294,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>47.7</v>
@@ -1323,15 +1317,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>34</v>
@@ -1346,15 +1340,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1369,15 +1363,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>34</v>
@@ -1392,15 +1386,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>59.2</v>
@@ -1415,15 +1409,15 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>64</v>
@@ -1438,15 +1432,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>242.5</v>
@@ -1461,15 +1455,15 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>89</v>
@@ -1484,15 +1478,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>119</v>
@@ -1507,15 +1501,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>116</v>
@@ -1530,15 +1524,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>45</v>
@@ -1553,15 +1547,15 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>200</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>128</v>
@@ -1576,15 +1570,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -1599,15 +1593,15 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>149</v>
@@ -1622,15 +1616,15 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <v>144</v>
@@ -1645,15 +1639,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>74</v>
@@ -1668,15 +1662,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <v>200</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>548</v>
@@ -1691,15 +1685,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27">
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>154</v>
@@ -1714,15 +1708,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>114</v>
@@ -1737,15 +1731,15 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>120</v>
@@ -1760,15 +1754,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>120</v>
@@ -1783,15 +1777,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -1806,15 +1800,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>205</v>
@@ -1829,15 +1823,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>28</v>
@@ -1852,15 +1846,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>280</v>
@@ -1875,15 +1869,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>13</v>
@@ -1898,15 +1892,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36">
         <v>64</v>
@@ -1921,15 +1915,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>13</v>
@@ -1944,15 +1938,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <v>22</v>
@@ -1967,15 +1961,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>13</v>
@@ -1990,15 +1984,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40">
         <v>34</v>
@@ -2013,15 +2007,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41">
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41">
         <v>25</v>
@@ -2036,15 +2030,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42">
         <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42">
         <v>86</v>
@@ -2059,15 +2053,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43">
         <v>20</v>
@@ -2082,15 +2076,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44">
         <v>24</v>
@@ -2105,15 +2099,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45">
         <v>50</v>
@@ -2128,15 +2122,15 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46">
         <v>5</v>
@@ -2151,15 +2145,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0.5</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47">
         <v>65</v>
@@ -2174,15 +2168,15 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48">
         <v>89</v>
@@ -2197,15 +2191,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49">
         <v>100</v>
@@ -2220,15 +2214,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50">
         <v>24</v>
@@ -2243,15 +2237,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D51">
         <v>6</v>
@@ -2266,15 +2260,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52">
         <v>45</v>
@@ -2289,15 +2283,15 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D53">
         <v>35</v>
@@ -2312,15 +2306,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54">
         <v>34</v>
@@ -2335,15 +2329,15 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D55">
         <v>50</v>
@@ -2358,15 +2352,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56">
         <v>234.7</v>
@@ -2381,15 +2375,15 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57">
         <v>350.4</v>
@@ -2404,15 +2398,15 @@
         <v>15.25</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D58">
         <v>95.1</v>
@@ -2427,15 +2421,15 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59">
         <v>500</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D59">
         <v>215</v>
@@ -2450,15 +2444,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D60">
         <v>162</v>
@@ -2473,15 +2467,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61">
         <v>210</v>
@@ -2493,29 +2487,6 @@
         <v>26</v>
       </c>
       <c r="G61">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>73</v>
-      </c>
-      <c r="D62">
-        <v>211</v>
-      </c>
-      <c r="E62">
-        <v>21</v>
-      </c>
-      <c r="F62">
-        <v>26</v>
-      </c>
-      <c r="G62">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
(1) Convert FoodDictionary.xlsx to Heb (2) Beta version for streamlit (3) TODO: input from user and last update
</commit_message>
<xml_diff>
--- a/Nutrition/FoodDictionary.xlsx
+++ b/Nutrition/FoodDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kobi Cohen\PycharmProjects\NutritionLog\Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E39FC-1E89-45CF-B4A4-351D245E3D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03B358E-A0CA-41A0-BBBF-9A7CBAAE50E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="750" windowWidth="17295" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17295" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodDictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
   <si>
     <t>Food</t>
   </si>
@@ -40,202 +40,292 @@
     <t>Fats</t>
   </si>
   <si>
-    <t>Bread</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>Tortilla</t>
-  </si>
-  <si>
-    <t>Black peas</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>Peanut butter</t>
-  </si>
-  <si>
-    <t>Tsp</t>
-  </si>
-  <si>
-    <t>Butter</t>
-  </si>
-  <si>
-    <t>Olive oil</t>
-  </si>
-  <si>
-    <t>sp</t>
-  </si>
-  <si>
-    <t>Oil spray</t>
-  </si>
-  <si>
-    <t>Teryaki souce</t>
-  </si>
-  <si>
-    <t>Honey</t>
-  </si>
-  <si>
-    <t>Tehinee</t>
-  </si>
-  <si>
-    <t>Almonds</t>
-  </si>
-  <si>
-    <t>Peanuts</t>
-  </si>
-  <si>
-    <t>Dark Chocolate</t>
-  </si>
-  <si>
-    <t>Cream Chease 0.5%</t>
-  </si>
-  <si>
-    <t>Cottage Chease</t>
-  </si>
-  <si>
-    <t>Ricotta Chease</t>
-  </si>
-  <si>
-    <t>Salted Chease</t>
-  </si>
-  <si>
-    <t>Yogurt pro 0%</t>
-  </si>
-  <si>
-    <t>Emmental Chease</t>
-  </si>
-  <si>
-    <t>Milk 2%</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>Pastrami</t>
-  </si>
-  <si>
-    <t>Salmon fish</t>
-  </si>
-  <si>
-    <t>Tuna fish</t>
-  </si>
-  <si>
-    <t>Sea bass fish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrecote </t>
-  </si>
-  <si>
-    <t>Minutte steak</t>
-  </si>
-  <si>
-    <t>Chicken breast</t>
-  </si>
-  <si>
-    <t>Chuncked tuna</t>
-  </si>
-  <si>
-    <t>Protein shake</t>
-  </si>
-  <si>
-    <t>egg</t>
-  </si>
-  <si>
-    <t>Smoked salmon</t>
-  </si>
-  <si>
-    <t>Red pepper</t>
-  </si>
-  <si>
-    <t>avocado</t>
-  </si>
-  <si>
-    <t>champignon mushrooms</t>
-  </si>
-  <si>
-    <t>carotte</t>
-  </si>
-  <si>
-    <t>lettuce</t>
-  </si>
-  <si>
-    <t>tomato</t>
-  </si>
-  <si>
-    <t>cucumber</t>
-  </si>
-  <si>
-    <t>broccoli</t>
-  </si>
-  <si>
-    <t>pumkin</t>
-  </si>
-  <si>
-    <t>sweet potato</t>
-  </si>
-  <si>
-    <t>courgette</t>
-  </si>
-  <si>
-    <t>eggplant</t>
-  </si>
-  <si>
-    <t>onion</t>
-  </si>
-  <si>
-    <t>spinach</t>
-  </si>
-  <si>
-    <t>mango</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>pomme grenade</t>
-  </si>
-  <si>
-    <t>strawberry</t>
-  </si>
-  <si>
-    <t>date fruit</t>
-  </si>
-  <si>
-    <t>peach</t>
-  </si>
-  <si>
-    <t>passion fruit</t>
-  </si>
-  <si>
-    <t>green apple</t>
-  </si>
-  <si>
-    <t>omlette</t>
-  </si>
-  <si>
-    <t>my proteined breakfast</t>
-  </si>
-  <si>
-    <t>salad</t>
-  </si>
-  <si>
-    <t>beer</t>
-  </si>
-  <si>
-    <t>wine</t>
-  </si>
-  <si>
-    <t>protein bar</t>
-  </si>
-  <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>לחם קל (פרוסה)</t>
+  </si>
+  <si>
+    <t>פריכיות</t>
+  </si>
+  <si>
+    <t>פסטה כוסמין קמח מלא</t>
+  </si>
+  <si>
+    <t>אורז בסמטי מלא אורגני</t>
+  </si>
+  <si>
+    <t>זרעי פשתן (כפית)</t>
+  </si>
+  <si>
+    <t>קינואה</t>
+  </si>
+  <si>
+    <t>בורגול</t>
+  </si>
+  <si>
+    <t>פיתה קלה מקמח מלא</t>
+  </si>
+  <si>
+    <t>טורטייה</t>
+  </si>
+  <si>
+    <t>עדשים שחורות</t>
+  </si>
+  <si>
+    <t>כוסמת</t>
+  </si>
+  <si>
+    <t>חמאת בוטנים</t>
+  </si>
+  <si>
+    <t>חמאה</t>
+  </si>
+  <si>
+    <t>שמן זית</t>
+  </si>
+  <si>
+    <t>שמן ספריי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רוטב טריאקי </t>
+  </si>
+  <si>
+    <t>דבש (כף 15 ג)</t>
+  </si>
+  <si>
+    <t>קטשופ</t>
+  </si>
+  <si>
+    <t>טחינה (כפית 5 גר)</t>
+  </si>
+  <si>
+    <t>שקדים</t>
+  </si>
+  <si>
+    <t>בוטנים - 5 בוטנים = 6 ג</t>
+  </si>
+  <si>
+    <t>פיסטוקים</t>
+  </si>
+  <si>
+    <t>קשיו</t>
+  </si>
+  <si>
+    <t>שוקולד מריר 90%</t>
+  </si>
+  <si>
+    <t>גבינה לבנה 0.5%</t>
+  </si>
+  <si>
+    <t>קוטג' 3% - גביע</t>
+  </si>
+  <si>
+    <t>קוטג' 5% שטראוס - 250 ג</t>
+  </si>
+  <si>
+    <t>ריקוטה 5% גד</t>
+  </si>
+  <si>
+    <t>בולגרית פיראוס 5%</t>
+  </si>
+  <si>
+    <t>יוגורט 0%</t>
+  </si>
+  <si>
+    <t>דנונה פרו 0%</t>
+  </si>
+  <si>
+    <t>אקטיביה 1.5%</t>
+  </si>
+  <si>
+    <t>גבינה צהובה 5%</t>
+  </si>
+  <si>
+    <t>חלב פרו 2% כוס=200מל</t>
+  </si>
+  <si>
+    <t>3 פרוסות פסרטמה</t>
+  </si>
+  <si>
+    <t>סטייק אנטריקוט</t>
+  </si>
+  <si>
+    <t>סינטה בקר (חבילה 250ג)</t>
+  </si>
+  <si>
+    <t>חזה עוף 100 גרם</t>
+  </si>
+  <si>
+    <t>טונה במים</t>
+  </si>
+  <si>
+    <t>שייק חלבון</t>
+  </si>
+  <si>
+    <t>ביצה קשה</t>
+  </si>
+  <si>
+    <t>סלומון מעושן - 100 ג'</t>
+  </si>
+  <si>
+    <t>פלפל אדום</t>
+  </si>
+  <si>
+    <t>אבוקדו בינוני</t>
+  </si>
+  <si>
+    <t>פטריות 50 גר'</t>
+  </si>
+  <si>
+    <t>גזר מגורד - מנה ממוצעת 50ג</t>
+  </si>
+  <si>
+    <t>חסה</t>
+  </si>
+  <si>
+    <t>עגבניה</t>
+  </si>
+  <si>
+    <t>מלפפון</t>
+  </si>
+  <si>
+    <t>ברוקלי</t>
+  </si>
+  <si>
+    <t>דלעת</t>
+  </si>
+  <si>
+    <t>בטטה</t>
+  </si>
+  <si>
+    <t>קישוא</t>
+  </si>
+  <si>
+    <t>חציל</t>
+  </si>
+  <si>
+    <t>שעועית לבנה מבושלת</t>
+  </si>
+  <si>
+    <t>בצל</t>
+  </si>
+  <si>
+    <t>תרד</t>
+  </si>
+  <si>
+    <t>חצי מנגו</t>
+  </si>
+  <si>
+    <t>בננה</t>
+  </si>
+  <si>
+    <t>תפוז</t>
+  </si>
+  <si>
+    <t>רימון</t>
+  </si>
+  <si>
+    <t>תות בינוני</t>
+  </si>
+  <si>
+    <t>תמר</t>
+  </si>
+  <si>
+    <t>אפרסק</t>
+  </si>
+  <si>
+    <t>אגס</t>
+  </si>
+  <si>
+    <t>פומלה</t>
+  </si>
+  <si>
+    <t>פסיפלורה</t>
+  </si>
+  <si>
+    <t>פטל שחור מוקפא</t>
+  </si>
+  <si>
+    <t>תות שדה מוקפא</t>
+  </si>
+  <si>
+    <t>תפוח ירוק</t>
+  </si>
+  <si>
+    <t>חביתה</t>
+  </si>
+  <si>
+    <t>א. בוקר חלבונית :)</t>
+  </si>
+  <si>
+    <t>צלי בקר</t>
+  </si>
+  <si>
+    <t>סלט ירקות</t>
+  </si>
+  <si>
+    <t>חריימה</t>
+  </si>
+  <si>
+    <t>יין</t>
+  </si>
+  <si>
+    <t>חטיף חלבון</t>
+  </si>
+  <si>
+    <t>חלבה</t>
+  </si>
+  <si>
+    <t>קרם קוקוס</t>
+  </si>
+  <si>
+    <t>נודלס מבושל</t>
+  </si>
+  <si>
+    <t>יחידות</t>
+  </si>
+  <si>
+    <t>כף</t>
+  </si>
+  <si>
+    <t>גרם</t>
+  </si>
+  <si>
+    <t>כפית</t>
+  </si>
+  <si>
+    <t>יחידה</t>
+  </si>
+  <si>
+    <t>מנה</t>
+  </si>
+  <si>
+    <t>גביע</t>
+  </si>
+  <si>
+    <t>כוס</t>
+  </si>
+  <si>
+    <t>פילה</t>
+  </si>
+  <si>
+    <t>סקופ</t>
+  </si>
+  <si>
+    <t>מ"ל</t>
+  </si>
+  <si>
+    <t>קוטג' 1% - גביע</t>
+  </si>
+  <si>
+    <t>דג מוסר ים (פילה ~ 200 גרם)</t>
+  </si>
+  <si>
+    <t>דג לברק (פילה ~ 200 גרם)</t>
+  </si>
+  <si>
+    <t>דג סלמון (פילה ~ 200 גרם)</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1112,13 +1202,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>65</v>
@@ -1138,22 +1228,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D3">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="E3">
-        <v>3.46</v>
+        <v>1.7</v>
       </c>
       <c r="F3">
-        <v>19</v>
+        <v>15.3</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1164,177 +1254,177 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D4">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="F4">
-        <v>20</v>
+        <v>27.5</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D5">
-        <v>30.85</v>
+        <v>84</v>
       </c>
       <c r="E5">
-        <v>1.4</v>
+        <v>3.1</v>
       </c>
       <c r="F5">
-        <v>4.1333333330000004</v>
+        <v>19.2</v>
       </c>
       <c r="G5">
-        <v>2.4500000000000002</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D6">
-        <v>745</v>
+        <v>162</v>
       </c>
       <c r="E6">
-        <v>0.7</v>
+        <v>3.8</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G6">
-        <v>82</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="G7">
-        <v>7.4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D8">
-        <v>1.5</v>
+        <v>120</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>21.3</v>
       </c>
       <c r="G8">
-        <v>0.2</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D9">
-        <v>8.34</v>
+        <v>83</v>
       </c>
       <c r="E9">
-        <v>0.156</v>
+        <v>3.08</v>
       </c>
       <c r="F9">
-        <v>1.5</v>
+        <v>19</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D10">
-        <v>47.7</v>
+        <v>83</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>5.42</v>
       </c>
       <c r="F10">
-        <v>11.925000000000001</v>
+        <v>9.66</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>127</v>
+      </c>
+      <c r="E11">
+        <v>3.46</v>
+      </c>
+      <c r="F11">
         <v>19</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>34</v>
-      </c>
-      <c r="E11">
-        <v>1.2</v>
-      </c>
-      <c r="F11">
-        <v>0.65</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -1342,183 +1432,183 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12">
+        <v>114</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>0.2</v>
-      </c>
-      <c r="F12">
-        <v>0.2</v>
-      </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D13">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="E13">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="D14">
-        <v>59.2</v>
+        <v>30.85</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="F14">
-        <v>1.4</v>
+        <v>4.1333333333333337</v>
       </c>
       <c r="G14">
-        <v>5.5</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D15">
-        <v>64</v>
+        <v>745</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F15">
-        <v>4.8</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0.5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D16">
-        <v>242.5</v>
+        <v>66</v>
       </c>
       <c r="E16">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>6.75</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>12.5</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="D17">
-        <v>89</v>
+        <v>1.5</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="D18">
-        <v>119</v>
+        <v>8.34</v>
       </c>
       <c r="E18">
-        <v>18</v>
+        <v>0.156</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D19">
-        <v>116</v>
+        <v>47.7</v>
       </c>
       <c r="E19">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>6.7</v>
+        <v>11.925000000000001</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1526,968 +1616,1543 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D20">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="E20">
-        <v>8.5</v>
+        <v>0.3</v>
       </c>
       <c r="F20">
-        <v>0.05</v>
+        <v>3.8</v>
       </c>
       <c r="G20">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="E21">
-        <v>12</v>
+        <v>1.2</v>
       </c>
       <c r="F21">
-        <v>11.2</v>
+        <v>0.65</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D22">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>10.6</v>
+        <v>0.2</v>
       </c>
       <c r="F22">
-        <v>2.6</v>
+        <v>0.2</v>
       </c>
       <c r="G22">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D23">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="E23">
-        <v>25.6</v>
+        <v>1.5</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>4.4000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
         <v>33</v>
       </c>
-      <c r="B24">
-        <v>100</v>
-      </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D24">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="E24">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D25">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>18</v>
+        <v>0.3</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D26">
-        <v>548</v>
+        <v>59.2</v>
       </c>
       <c r="E26">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="G26">
-        <v>45</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B27">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="D27">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="E27">
-        <v>20</v>
+        <v>23.4</v>
       </c>
       <c r="F27">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>100</v>
       </c>
       <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28">
+        <v>64</v>
+      </c>
+      <c r="E28">
         <v>10</v>
       </c>
-      <c r="D28">
-        <v>114</v>
-      </c>
-      <c r="E28">
-        <v>21</v>
-      </c>
       <c r="F28">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="G28">
-        <v>2.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D29">
-        <v>120</v>
+        <v>192.5</v>
       </c>
       <c r="E29">
-        <v>26</v>
+        <v>27.5</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D30">
-        <v>120</v>
+        <v>242.5</v>
       </c>
       <c r="E30">
-        <v>24</v>
+        <v>25.5</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>6.75</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31">
+        <v>89</v>
+      </c>
+      <c r="E31">
         <v>7</v>
       </c>
-      <c r="D31">
-        <v>90</v>
-      </c>
-      <c r="E31">
-        <v>7.3</v>
-      </c>
       <c r="F31">
-        <v>0.6</v>
+        <v>7</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D32">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="E32">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G32">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D33">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33">
-        <v>7.5</v>
+        <v>9.6</v>
       </c>
       <c r="G33">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D34">
-        <v>280</v>
+        <v>116</v>
       </c>
       <c r="E34">
-        <v>3.5</v>
+        <v>21</v>
       </c>
       <c r="F34">
-        <v>15</v>
+        <v>6.7</v>
       </c>
       <c r="G34">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B35">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="D35">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G35">
-        <v>0.1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36">
         <v>45</v>
       </c>
-      <c r="B36">
-        <v>100</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36">
-        <v>64</v>
-      </c>
       <c r="E36">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="F36">
-        <v>13</v>
+        <v>0.05</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D37">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="E37">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="F37">
-        <v>2.2999999999999998</v>
+        <v>11.2</v>
       </c>
       <c r="G37">
-        <v>0.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D38">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>10.6</v>
       </c>
       <c r="F38">
-        <v>4.3</v>
+        <v>2.6</v>
       </c>
       <c r="G38">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D39">
-        <v>13</v>
+        <v>300</v>
       </c>
       <c r="E39">
-        <v>0.7</v>
+        <v>51.2</v>
       </c>
       <c r="F39">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>0.1</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B40">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="D40">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>0.5</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41">
+        <v>148</v>
+      </c>
+      <c r="E41">
+        <v>36</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>10</v>
-      </c>
-      <c r="D41">
-        <v>25</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>6.5</v>
-      </c>
-      <c r="G41">
-        <v>0.1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B42">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D42">
-        <v>86</v>
+        <v>548</v>
       </c>
       <c r="E42">
-        <v>1.6</v>
+        <v>35</v>
       </c>
       <c r="F42">
-        <v>20.12</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>0.05</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D43">
+        <v>154</v>
+      </c>
+      <c r="E43">
         <v>20</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
       <c r="F43">
-        <v>4.3</v>
+        <v>0.5</v>
       </c>
       <c r="G43">
-        <v>0.3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D44">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>0.2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="D45">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E45">
-        <v>1.4</v>
+        <v>26</v>
       </c>
       <c r="F45">
-        <v>11.7</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>0.125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E46">
-        <v>0.6</v>
+        <v>24</v>
       </c>
       <c r="F46">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="D47">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E47">
-        <v>0.5</v>
+        <v>7.3</v>
       </c>
       <c r="F47">
-        <v>17</v>
+        <v>0.6</v>
       </c>
       <c r="G47">
-        <v>0.6</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D48">
-        <v>89</v>
+        <v>205</v>
       </c>
       <c r="E48">
-        <v>1.1000000000000001</v>
+        <v>21</v>
       </c>
       <c r="F48">
-        <v>22.8</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <v>0.3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D49">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>25</v>
+        <v>7.5</v>
       </c>
       <c r="G49">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50">
+        <v>280</v>
+      </c>
+      <c r="E50">
+        <v>3.5</v>
+      </c>
+      <c r="F50">
         <v>15</v>
       </c>
-      <c r="D50">
-        <v>24</v>
-      </c>
-      <c r="E50">
-        <v>0.5</v>
-      </c>
-      <c r="F50">
-        <v>5.5</v>
-      </c>
       <c r="G50">
-        <v>0.4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E51">
-        <v>0.14000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G51">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D52">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E52">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F52">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G52">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D53">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E53">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="F53">
-        <v>8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G53">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D54">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E54">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F54">
-        <v>8.1999999999999993</v>
+        <v>4.3</v>
       </c>
       <c r="G54">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D55">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E55">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F55">
-        <v>13.5</v>
+        <v>2.8</v>
       </c>
       <c r="G55">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56">
+        <v>34</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
         <v>7</v>
       </c>
-      <c r="D56">
-        <v>234.7</v>
-      </c>
-      <c r="E56">
-        <v>21</v>
-      </c>
-      <c r="F56">
-        <v>3.35</v>
-      </c>
       <c r="G56">
-        <v>14.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D57">
-        <v>350.4</v>
+        <v>25</v>
       </c>
       <c r="E57">
-        <v>46.9</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>3.45</v>
+        <v>6.5</v>
       </c>
       <c r="G57">
-        <v>15.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D58">
-        <v>95.1</v>
+        <v>86</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>1.6</v>
       </c>
       <c r="F58">
-        <v>16.8</v>
+        <v>20.12</v>
       </c>
       <c r="G58">
-        <v>0.72</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="D59">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="E59">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="F59">
-        <v>18</v>
+        <v>4.3</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D60">
-        <v>162</v>
+        <v>24</v>
       </c>
       <c r="E60">
-        <v>0.14000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61">
+        <v>139</v>
+      </c>
+      <c r="E61">
+        <v>9.73</v>
+      </c>
+      <c r="F61">
+        <v>25</v>
+      </c>
+      <c r="G61">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>1.4</v>
+      </c>
+      <c r="F62">
+        <v>11.7</v>
+      </c>
+      <c r="G62">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>0.6</v>
+      </c>
+      <c r="F63">
+        <v>0.5</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>0.5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64">
+        <v>65</v>
+      </c>
+      <c r="E64">
+        <v>0.5</v>
+      </c>
+      <c r="F64">
+        <v>17</v>
+      </c>
+      <c r="G64">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65">
+        <v>89</v>
+      </c>
+      <c r="E65">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F65">
+        <v>22.8</v>
+      </c>
+      <c r="G65">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>25</v>
+      </c>
+      <c r="G66">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67">
+        <v>24</v>
+      </c>
+      <c r="E67">
+        <v>0.5</v>
+      </c>
+      <c r="F67">
+        <v>5.5</v>
+      </c>
+      <c r="G67">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F68">
+        <v>1.5</v>
+      </c>
+      <c r="G68">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D69">
+        <v>45</v>
+      </c>
+      <c r="E69">
+        <v>0.3</v>
+      </c>
+      <c r="F69">
+        <v>11</v>
+      </c>
+      <c r="G69">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70">
+        <v>35</v>
+      </c>
+      <c r="E70">
+        <v>0.5</v>
+      </c>
+      <c r="F70">
+        <v>8</v>
+      </c>
+      <c r="G70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>87</v>
+      </c>
+      <c r="D71">
+        <v>58</v>
+      </c>
+      <c r="E71">
+        <v>0.4</v>
+      </c>
+      <c r="F71">
+        <v>15.5</v>
+      </c>
+      <c r="G71">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>87</v>
+      </c>
+      <c r="D72">
+        <v>95</v>
+      </c>
+      <c r="E72">
+        <v>1.9</v>
+      </c>
+      <c r="F72">
+        <v>24</v>
+      </c>
+      <c r="G72">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73">
+        <v>34</v>
+      </c>
+      <c r="E73">
+        <v>0.8</v>
+      </c>
+      <c r="F73">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G73">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74">
+        <v>57</v>
+      </c>
+      <c r="E74">
+        <v>1.7</v>
+      </c>
+      <c r="F74">
+        <v>8.6</v>
+      </c>
+      <c r="G74">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <v>100</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75">
+        <v>33</v>
+      </c>
+      <c r="E75">
+        <v>0.8</v>
+      </c>
+      <c r="F75">
+        <v>5.7</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>87</v>
+      </c>
+      <c r="D76">
+        <v>50</v>
+      </c>
+      <c r="E76">
+        <v>0.3</v>
+      </c>
+      <c r="F76">
+        <v>13.5</v>
+      </c>
+      <c r="G76">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77">
+        <v>234.7</v>
+      </c>
+      <c r="E77">
+        <v>21</v>
+      </c>
+      <c r="F77">
+        <v>3.3499999999999996</v>
+      </c>
+      <c r="G77">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>87</v>
+      </c>
+      <c r="D78">
+        <v>350.4</v>
+      </c>
+      <c r="E78">
+        <v>46.9</v>
+      </c>
+      <c r="F78">
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="G78">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>87</v>
+      </c>
+      <c r="D79">
+        <v>297</v>
+      </c>
+      <c r="E79">
+        <v>33</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>91</v>
+      </c>
+      <c r="D80">
+        <v>95.1</v>
+      </c>
+      <c r="E80">
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="F80">
+        <v>16.8</v>
+      </c>
+      <c r="G80">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>87</v>
+      </c>
+      <c r="D81">
+        <v>372</v>
+      </c>
+      <c r="E81">
+        <v>43</v>
+      </c>
+      <c r="F81">
+        <v>8</v>
+      </c>
+      <c r="G81">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>87</v>
+      </c>
+      <c r="D82">
+        <v>297</v>
+      </c>
+      <c r="E82">
+        <v>33</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83">
+        <v>162</v>
+      </c>
+      <c r="E83">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F83">
+        <v>4</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84">
+        <v>210</v>
+      </c>
+      <c r="E84">
+        <v>20</v>
+      </c>
+      <c r="F84">
+        <v>26</v>
+      </c>
+      <c r="G84">
         <v>7</v>
       </c>
-      <c r="D61">
-        <v>210</v>
-      </c>
-      <c r="E61">
-        <v>20</v>
-      </c>
-      <c r="F61">
-        <v>26</v>
-      </c>
-      <c r="G61">
-        <v>7</v>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>100</v>
+      </c>
+      <c r="C85" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85">
+        <v>388</v>
+      </c>
+      <c r="E85">
+        <v>10</v>
+      </c>
+      <c r="F85">
+        <v>45</v>
+      </c>
+      <c r="G85">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>100</v>
+      </c>
+      <c r="C86" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86">
+        <v>206</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86">
+        <v>2.92</v>
+      </c>
+      <c r="G86">
+        <v>20.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final stable version with streamlit
</commit_message>
<xml_diff>
--- a/Nutrition/FoodDictionary.xlsx
+++ b/Nutrition/FoodDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kobi Cohen\PycharmProjects\NutritionLog\Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03B358E-A0CA-41A0-BBBF-9A7CBAAE50E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79230551-82C0-47E9-9F0F-36FF996353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17295" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="585" windowWidth="15870" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodDictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
   <si>
     <t>Food</t>
   </si>
@@ -121,9 +121,6 @@
     <t>קוטג' 3% - גביע</t>
   </si>
   <si>
-    <t>קוטג' 5% שטראוס - 250 ג</t>
-  </si>
-  <si>
     <t>ריקוטה 5% גד</t>
   </si>
   <si>
@@ -145,18 +142,12 @@
     <t>חלב פרו 2% כוס=200מל</t>
   </si>
   <si>
-    <t>3 פרוסות פסרטמה</t>
-  </si>
-  <si>
     <t>סטייק אנטריקוט</t>
   </si>
   <si>
     <t>סינטה בקר (חבילה 250ג)</t>
   </si>
   <si>
-    <t>חזה עוף 100 גרם</t>
-  </si>
-  <si>
     <t>טונה במים</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>ביצה קשה</t>
   </si>
   <si>
-    <t>סלומון מעושן - 100 ג'</t>
-  </si>
-  <si>
     <t>פלפל אדום</t>
   </si>
   <si>
@@ -214,9 +202,6 @@
     <t>תרד</t>
   </si>
   <si>
-    <t>חצי מנגו</t>
-  </si>
-  <si>
     <t>בננה</t>
   </si>
   <si>
@@ -244,12 +229,6 @@
     <t>פסיפלורה</t>
   </si>
   <si>
-    <t>פטל שחור מוקפא</t>
-  </si>
-  <si>
-    <t>תות שדה מוקפא</t>
-  </si>
-  <si>
     <t>תפוח ירוק</t>
   </si>
   <si>
@@ -326,6 +305,30 @@
   </si>
   <si>
     <t>דג סלמון (פילה ~ 200 גרם)</t>
+  </si>
+  <si>
+    <t>קוטג' 5% - גביע</t>
+  </si>
+  <si>
+    <t>פרוסה</t>
+  </si>
+  <si>
+    <t>פסטרמה</t>
+  </si>
+  <si>
+    <t>חזה עוף</t>
+  </si>
+  <si>
+    <t>דג סלומון מעושן</t>
+  </si>
+  <si>
+    <t>מנגו</t>
+  </si>
+  <si>
+    <t>פירות קפואים: פטל שחור</t>
+  </si>
+  <si>
+    <t>פירות קפואים: תות שדה</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>65</v>
@@ -1231,7 +1234,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>77</v>
@@ -1254,7 +1257,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>149</v>
@@ -1271,13 +1274,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>84</v>
@@ -1300,7 +1303,7 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D6">
         <v>162</v>
@@ -1323,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -1346,7 +1349,7 @@
         <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>120</v>
@@ -1369,7 +1372,7 @@
         <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D9">
         <v>83</v>
@@ -1392,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>83</v>
@@ -1415,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D11">
         <v>127</v>
@@ -1438,7 +1441,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>114</v>
@@ -1461,7 +1464,7 @@
         <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D13">
         <v>92</v>
@@ -1484,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D14">
         <v>30.85</v>
@@ -1507,7 +1510,7 @@
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D15">
         <v>745</v>
@@ -1530,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>66</v>
@@ -1553,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D17">
         <v>1.5</v>
@@ -1576,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D18">
         <v>8.34</v>
@@ -1599,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D19">
         <v>47.7</v>
@@ -1622,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D20">
         <v>16</v>
@@ -1645,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D21">
         <v>34</v>
@@ -1668,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -1691,7 +1694,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D23">
         <v>34</v>
@@ -1714,7 +1717,7 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>184</v>
@@ -1737,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D25">
         <v>12</v>
@@ -1760,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D26">
         <v>59.2</v>
@@ -1777,13 +1780,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D27">
         <v>120</v>
@@ -1806,7 +1809,7 @@
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>64</v>
@@ -1829,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D29">
         <v>192.5</v>
@@ -1846,13 +1849,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <v>242.5</v>
@@ -1869,13 +1872,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D31">
         <v>89</v>
@@ -1892,13 +1895,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D32">
         <v>119</v>
@@ -1915,13 +1918,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D33">
         <v>78</v>
@@ -1938,13 +1941,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D34">
         <v>116</v>
@@ -1961,13 +1964,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D35">
         <v>118</v>
@@ -1984,13 +1987,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D36">
         <v>45</v>
@@ -2007,13 +2010,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D37">
         <v>128</v>
@@ -2030,13 +2033,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D38">
         <v>60</v>
@@ -2053,13 +2056,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D39">
         <v>300</v>
@@ -2076,13 +2079,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D40">
         <v>228</v>
@@ -2099,13 +2102,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D41">
         <v>148</v>
@@ -2122,13 +2125,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D42">
         <v>548</v>
@@ -2145,13 +2148,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D43">
         <v>154</v>
@@ -2168,13 +2171,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B44">
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D44">
         <v>114</v>
@@ -2191,13 +2194,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D45">
         <v>120</v>
@@ -2214,13 +2217,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D46">
         <v>120</v>
@@ -2237,13 +2240,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D47">
         <v>90</v>
@@ -2260,13 +2263,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B48">
         <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D48">
         <v>205</v>
@@ -2283,13 +2286,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D49">
         <v>28</v>
@@ -2306,13 +2309,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D50">
         <v>280</v>
@@ -2329,13 +2332,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D51">
         <v>13</v>
@@ -2352,13 +2355,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B52">
         <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D52">
         <v>64</v>
@@ -2375,13 +2378,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D53">
         <v>13</v>
@@ -2398,13 +2401,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D54">
         <v>22</v>
@@ -2421,13 +2424,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D55">
         <v>13</v>
@@ -2444,13 +2447,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B56">
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D56">
         <v>34</v>
@@ -2467,13 +2470,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B57">
         <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D57">
         <v>25</v>
@@ -2490,13 +2493,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B58">
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D58">
         <v>86</v>
@@ -2513,13 +2516,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D59">
         <v>20</v>
@@ -2536,13 +2539,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B60">
         <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D60">
         <v>24</v>
@@ -2559,13 +2562,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B61">
         <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D61">
         <v>139</v>
@@ -2582,13 +2585,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D62">
         <v>50</v>
@@ -2605,13 +2608,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B63">
         <v>50</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D63">
         <v>5</v>
@@ -2628,13 +2631,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B64">
         <v>0.5</v>
       </c>
       <c r="C64" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D64">
         <v>65</v>
@@ -2651,13 +2654,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D65">
         <v>89</v>
@@ -2674,13 +2677,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D66">
         <v>100</v>
@@ -2697,13 +2700,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D67">
         <v>24</v>
@@ -2720,13 +2723,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D68">
         <v>6</v>
@@ -2743,13 +2746,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D69">
         <v>45</v>
@@ -2766,13 +2769,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D70">
         <v>35</v>
@@ -2789,13 +2792,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D71">
         <v>58</v>
@@ -2812,13 +2815,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D72">
         <v>95</v>
@@ -2835,13 +2838,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D73">
         <v>34</v>
@@ -2858,13 +2861,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="B74">
         <v>100</v>
       </c>
       <c r="C74" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D74">
         <v>57</v>
@@ -2881,13 +2884,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B75">
         <v>100</v>
       </c>
       <c r="C75" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D75">
         <v>33</v>
@@ -2904,13 +2907,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D76">
         <v>50</v>
@@ -2927,13 +2930,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D77">
         <v>234.7</v>
@@ -2950,13 +2953,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D78">
         <v>350.4</v>
@@ -2973,13 +2976,13 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D79">
         <v>297</v>
@@ -2996,13 +2999,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D80">
         <v>95.1</v>
@@ -3019,13 +3022,13 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D81">
         <v>372</v>
@@ -3042,13 +3045,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D82">
         <v>297</v>
@@ -3065,13 +3068,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D83">
         <v>162</v>
@@ -3088,13 +3091,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D84">
         <v>210</v>
@@ -3111,13 +3114,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B85">
         <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D85">
         <v>388</v>
@@ -3134,13 +3137,13 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B86">
         <v>100</v>
       </c>
       <c r="C86" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D86">
         <v>206</v>

</xml_diff>

<commit_message>
added some comments and values to food-dictionary
</commit_message>
<xml_diff>
--- a/Nutrition/FoodDictionary.xlsx
+++ b/Nutrition/FoodDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kobi Cohen\PycharmProjects\NutritionLog\Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79230551-82C0-47E9-9F0F-36FF996353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFEF68F-D9B9-49AB-BDE5-4521722F9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="585" windowWidth="15870" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="900" windowWidth="9480" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodDictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="109">
   <si>
     <t>Food</t>
   </si>
@@ -115,9 +115,6 @@
     <t>שוקולד מריר 90%</t>
   </si>
   <si>
-    <t>גבינה לבנה 0.5%</t>
-  </si>
-  <si>
     <t>קוטג' 3% - גביע</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>יוגורט 0%</t>
   </si>
   <si>
-    <t>דנונה פרו 0%</t>
-  </si>
-  <si>
     <t>אקטיביה 1.5%</t>
   </si>
   <si>
@@ -329,6 +323,30 @@
   </si>
   <si>
     <t>פירות קפואים: תות שדה</t>
+  </si>
+  <si>
+    <t>חמוציות [גר]</t>
+  </si>
+  <si>
+    <t>גבינת סקי 5% [גרם]</t>
+  </si>
+  <si>
+    <t>כרישה [גרם]</t>
+  </si>
+  <si>
+    <t>אספרגוס [גרם]</t>
+  </si>
+  <si>
+    <t>תירס [קלח]</t>
+  </si>
+  <si>
+    <t>גבינת סקי 0.5% [גרם]</t>
+  </si>
+  <si>
+    <t>יוגורט דנונה פרו 0%</t>
+  </si>
+  <si>
+    <t>יוגורט 3%</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>65</v>
@@ -1234,7 +1252,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>77</v>
@@ -1257,7 +1275,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4">
         <v>149</v>
@@ -1274,13 +1292,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>84</v>
@@ -1303,7 +1321,7 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>162</v>
@@ -1326,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -1349,7 +1367,7 @@
         <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8">
         <v>120</v>
@@ -1372,7 +1390,7 @@
         <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9">
         <v>83</v>
@@ -1395,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D10">
         <v>83</v>
@@ -1418,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11">
         <v>127</v>
@@ -1441,7 +1459,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12">
         <v>114</v>
@@ -1464,7 +1482,7 @@
         <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13">
         <v>92</v>
@@ -1487,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>30.85</v>
@@ -1510,7 +1528,7 @@
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15">
         <v>745</v>
@@ -1533,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>66</v>
@@ -1556,7 +1574,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17">
         <v>1.5</v>
@@ -1579,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18">
         <v>8.34</v>
@@ -1602,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19">
         <v>47.7</v>
@@ -1625,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20">
         <v>16</v>
@@ -1648,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21">
         <v>34</v>
@@ -1671,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -1694,7 +1712,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23">
         <v>34</v>
@@ -1717,7 +1735,7 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24">
         <v>184</v>
@@ -1740,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>12</v>
@@ -1763,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26">
         <v>59.2</v>
@@ -1780,13 +1798,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27">
         <v>120</v>
@@ -1803,13 +1821,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B28">
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28">
         <v>64</v>
@@ -1826,13 +1844,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29">
         <v>192.5</v>
@@ -1849,13 +1867,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30">
         <v>242.5</v>
@@ -1872,13 +1890,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D31">
         <v>89</v>
@@ -1895,13 +1913,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32">
         <v>119</v>
@@ -1918,13 +1936,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33">
         <v>78</v>
@@ -1941,53 +1959,53 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="E34">
-        <v>21</v>
+        <v>10.4</v>
       </c>
       <c r="F34">
-        <v>6.7</v>
+        <v>9</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E35">
-        <v>10.199999999999999</v>
+        <v>21</v>
       </c>
       <c r="F35">
-        <v>8.8000000000000007</v>
+        <v>6.7</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1996,243 +2014,243 @@
         <v>84</v>
       </c>
       <c r="D36">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E36">
-        <v>8.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F36">
-        <v>0.05</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G36">
-        <v>1.25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D37">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="F37">
-        <v>11.2</v>
+        <v>0.05</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D38">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="E38">
-        <v>10.6</v>
+        <v>12</v>
       </c>
       <c r="F38">
-        <v>2.6</v>
+        <v>11.2</v>
       </c>
       <c r="G38">
-        <v>0.7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
         <v>94</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
       <c r="D39">
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="E39">
-        <v>51.2</v>
+        <v>10.6</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="G39">
-        <v>8.8000000000000007</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D40">
-        <v>228</v>
+        <v>300</v>
       </c>
       <c r="E40">
-        <v>38</v>
+        <v>51.2</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>7.4</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D41">
-        <v>148</v>
+        <v>228</v>
       </c>
       <c r="E41">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>10</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B42">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D42">
-        <v>548</v>
+        <v>148</v>
       </c>
       <c r="E42">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43">
-        <v>154</v>
+        <v>548</v>
       </c>
       <c r="E43">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F43">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="B44">
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D44">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="E44">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G44">
-        <v>2.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D45">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E45">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D46">
         <v>120</v>
       </c>
       <c r="E46">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2240,574 +2258,574 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D47">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E47">
-        <v>7.3</v>
+        <v>24</v>
       </c>
       <c r="F47">
-        <v>0.6</v>
+        <v>4</v>
       </c>
       <c r="G47">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="B48">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="D48">
-        <v>205</v>
+        <v>90</v>
       </c>
       <c r="E48">
-        <v>21</v>
+        <v>7.3</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G48">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
         <v>80</v>
       </c>
       <c r="D49">
-        <v>28</v>
+        <v>205</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F49">
-        <v>7.5</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>0.3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D50">
-        <v>280</v>
+        <v>28</v>
       </c>
       <c r="E50">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="F50">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="G50">
-        <v>26</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D51">
-        <v>13</v>
+        <v>280</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G51">
-        <v>0.1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B52">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D52">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
         <v>80</v>
       </c>
       <c r="D53">
+        <v>64</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
         <v>13</v>
       </c>
-      <c r="E53">
-        <v>1.2</v>
-      </c>
-      <c r="F53">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="G53">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D54">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F54">
-        <v>4.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G54">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D55">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E55">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F55">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
       <c r="G55">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B56">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D56">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E56">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="F56">
-        <v>7</v>
+        <v>2.8</v>
       </c>
       <c r="G56">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B57">
         <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D57">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="G57">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B58">
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D58">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E58">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="F58">
-        <v>20.12</v>
+        <v>6.5</v>
       </c>
       <c r="G58">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D59">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F59">
-        <v>4.3</v>
+        <v>20.12</v>
       </c>
       <c r="G59">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B60">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
         <v>82</v>
       </c>
       <c r="D60">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60">
-        <v>6</v>
+        <v>4.3</v>
       </c>
       <c r="G60">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B61">
         <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D61">
-        <v>139</v>
+        <v>24</v>
       </c>
       <c r="E61">
-        <v>9.73</v>
+        <v>1</v>
       </c>
       <c r="F61">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G61">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D62">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="E62">
-        <v>1.4</v>
+        <v>9.73</v>
       </c>
       <c r="F62">
-        <v>11.7</v>
+        <v>25</v>
       </c>
       <c r="G62">
-        <v>0.125</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B63">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
         <v>82</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E63">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F63">
-        <v>0.5</v>
+        <v>11.7</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B64">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
         <v>80</v>
       </c>
       <c r="D64">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="E64">
+        <v>0.6</v>
+      </c>
+      <c r="F64">
         <v>0.5</v>
       </c>
-      <c r="F64">
-        <v>17</v>
-      </c>
       <c r="G64">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D65">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="E65">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F65">
-        <v>22.8</v>
+        <v>17</v>
       </c>
       <c r="G65">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D66">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F66">
-        <v>25</v>
+        <v>22.8</v>
       </c>
       <c r="G66">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D67">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="E67">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F67">
-        <v>5.5</v>
+        <v>25</v>
       </c>
       <c r="G67">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E68">
-        <v>0.14000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F68">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="G68">
-        <v>0.06</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D69">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E69">
-        <v>0.3</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F69">
-        <v>11</v>
+        <v>1.5</v>
       </c>
       <c r="G69">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D70">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E70">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="F70">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G70">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D71">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="E71">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F71">
-        <v>15.5</v>
+        <v>8</v>
       </c>
       <c r="G71">
         <v>0.1</v>
@@ -2815,22 +2833,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D72">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="E72">
-        <v>1.9</v>
+        <v>0.4</v>
       </c>
       <c r="F72">
-        <v>24</v>
+        <v>15.5</v>
       </c>
       <c r="G72">
         <v>0.1</v>
@@ -2838,209 +2856,209 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D73">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E73">
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="F73">
-        <v>8.1999999999999993</v>
+        <v>24</v>
       </c>
       <c r="G73">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="B74">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D74">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E74">
-        <v>1.7</v>
+        <v>0.8</v>
       </c>
       <c r="F74">
-        <v>8.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G74">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B75">
         <v>100</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D75">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="E75">
-        <v>0.8</v>
+        <v>1.7</v>
       </c>
       <c r="F75">
-        <v>5.7</v>
+        <v>8.6</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
         <v>80</v>
       </c>
       <c r="D76">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E76">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="F76">
-        <v>13.5</v>
+        <v>5.7</v>
       </c>
       <c r="G76">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D77">
-        <v>234.7</v>
+        <v>50</v>
       </c>
       <c r="E77">
-        <v>21</v>
+        <v>0.3</v>
       </c>
       <c r="F77">
-        <v>3.3499999999999996</v>
+        <v>13.5</v>
       </c>
       <c r="G77">
-        <v>14.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D78">
-        <v>350.4</v>
+        <v>234.7</v>
       </c>
       <c r="E78">
-        <v>46.9</v>
+        <v>21</v>
       </c>
       <c r="F78">
-        <v>3.4499999999999997</v>
+        <v>3.3499999999999996</v>
       </c>
       <c r="G78">
-        <v>15.25</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D79">
-        <v>297</v>
+        <v>350.4</v>
       </c>
       <c r="E79">
-        <v>33</v>
+        <v>46.9</v>
       </c>
       <c r="F79">
-        <v>3</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="G79">
-        <v>14</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D80">
-        <v>95.1</v>
+        <v>297</v>
       </c>
       <c r="E80">
-        <v>3.9999999999999996</v>
+        <v>33</v>
       </c>
       <c r="F80">
-        <v>16.8</v>
+        <v>3</v>
       </c>
       <c r="G80">
-        <v>0.72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D81">
-        <v>372</v>
+        <v>95.1</v>
       </c>
       <c r="E81">
-        <v>43</v>
+        <v>3.9999999999999996</v>
       </c>
       <c r="F81">
-        <v>8</v>
+        <v>16.8</v>
       </c>
       <c r="G81">
-        <v>18</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3051,111 +3069,249 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D82">
-        <v>297</v>
+        <v>372</v>
       </c>
       <c r="E82">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F82">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G82">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D83">
-        <v>162</v>
+        <v>297</v>
       </c>
       <c r="E83">
-        <v>0.14000000000000001</v>
+        <v>33</v>
       </c>
       <c r="F83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D84">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="E84">
-        <v>20</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F84">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G84">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B85">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
         <v>82</v>
       </c>
       <c r="D85">
-        <v>388</v>
+        <v>210</v>
       </c>
       <c r="E85">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F85">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="G85">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B86">
         <v>100</v>
       </c>
       <c r="C86" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D86">
+        <v>388</v>
+      </c>
+      <c r="E86">
+        <v>10</v>
+      </c>
+      <c r="F86">
+        <v>45</v>
+      </c>
+      <c r="G86">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>76</v>
+      </c>
+      <c r="B87">
+        <v>100</v>
+      </c>
+      <c r="C87" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87">
         <v>206</v>
       </c>
-      <c r="E86">
+      <c r="E87">
         <v>2</v>
       </c>
-      <c r="F86">
+      <c r="F87">
         <v>2.92</v>
       </c>
-      <c r="G86">
+      <c r="G87">
         <v>20.7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88">
+        <v>100</v>
+      </c>
+      <c r="C88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88">
+        <v>295</v>
+      </c>
+      <c r="E88">
+        <v>0.4</v>
+      </c>
+      <c r="F88">
+        <v>74</v>
+      </c>
+      <c r="G88">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>80</v>
+      </c>
+      <c r="D89">
+        <v>96</v>
+      </c>
+      <c r="E89">
+        <v>7.9</v>
+      </c>
+      <c r="F89">
+        <v>3.9</v>
+      </c>
+      <c r="G89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90">
+        <v>100</v>
+      </c>
+      <c r="C90" t="s">
+        <v>80</v>
+      </c>
+      <c r="D90">
+        <v>60</v>
+      </c>
+      <c r="E90">
+        <v>1.5</v>
+      </c>
+      <c r="F90">
+        <v>14</v>
+      </c>
+      <c r="G90">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91">
+        <v>100</v>
+      </c>
+      <c r="C91" t="s">
+        <v>80</v>
+      </c>
+      <c r="D91">
+        <v>20</v>
+      </c>
+      <c r="E91">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F91">
+        <v>3.2</v>
+      </c>
+      <c r="G91">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92">
+        <v>200</v>
+      </c>
+      <c r="E92">
+        <v>6.1420000000000003</v>
+      </c>
+      <c r="F92">
+        <v>46.454000000000001</v>
+      </c>
+      <c r="G92">
+        <v>2.3679999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>